<commit_message>
converted the functional paradigm to oops with encapsulation
</commit_message>
<xml_diff>
--- a/output/cow_gate.xlsx
+++ b/output/cow_gate.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -469,229 +469,139 @@
           <t>Cow &amp; Gate Follow-on Baby Milk Formula - Stage 2, 800gms, 6+months</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>&lt;div&gt;
+&lt;div&gt;
+&lt;ul&gt;
+&lt;li&gt;
+&lt;span&gt;&lt;span&gt;Nutritionally complete&lt;span&gt; Follow-on Baby Milk Formula&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;br&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;span &gt;Contains Lactose, Milk, Vegetable oils, Maltodextrin, Calcium &amp;amp; more&lt;/span&gt;&lt;/li&gt;
+&lt;li&gt;Suitable as a sole source of nutrition for growing babies&lt;/li&gt;
+&lt;li&gt;Nutritionally complete Fortified Milk Drink&lt;/li&gt;
+&lt;li&gt;Supports your baby’s normal growth and development.&lt;span style="font-size: 11.6667px;" data-mce-style="font-size: 11.6667px;"&gt; &lt;/span&gt;
+&lt;/li&gt;
+&lt;li&gt;Contains no artificial sweeteners &amp;amp; flavors&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&lt;span style="color: #1e2e7d;" &gt;&lt;strong&gt;Expiry Date :&lt;/strong&gt; 05/2024&lt;/span&gt;&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;&lt;span style="color: #1e2e7d;" &gt;Return&lt;/span&gt;&lt;span&gt;&lt;span style="color: #ff0000;" &gt;*&lt;/span&gt; &lt;/span&gt;&lt;/b&gt;: No&lt;/p&gt;
+&lt;p&gt;&lt;span&gt;&lt;b&gt;&lt;span style="color: #1e2e7d;" &gt;Replace / Exchange&lt;/span&gt;&lt;span style="color: #ff0000;" &gt;*&lt;/span&gt;&lt;/b&gt;&lt;/span&gt;&lt;span&gt; &lt;/span&gt;: No&lt;/p&gt;
+&lt;p&gt;&lt;span style="color: #1e2e7d;" &gt;&lt;strong&gt;Specifications:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt;Brand - Cow &amp;amp; Gate&lt;/li&gt;
+&lt;li&gt;Product - &lt;span &gt;Follow-on Baby Milk Formula&lt;/span&gt;
+&lt;/li&gt;
+&lt;li&gt;Age - 6+months&lt;/li&gt;
+&lt;li&gt;Grams - 800gms&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&lt;span style="color: #1e2e7d;" &gt;&lt;strong&gt;Instructions:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;/div&gt;
+&lt;ul&gt;
+&lt;li&gt;Consult Doctor before introducing&lt;span&gt; Follow-on Baby Milk Formula&lt;/span&gt;&lt;span &gt;&lt;span&gt; &lt;/span&gt;&lt;/span&gt;to your child&lt;/li&gt;
+&lt;li&gt;Do not use fewer scoops than directed&lt;/li&gt;
+&lt;li&gt;Store in cool air tight container&lt;/li&gt;
+&lt;li&gt;Please note : Mothers milk is always best for your baby&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Country of Origin: U.K&lt;/p&gt;
+&lt;p&gt;&lt;span style="color: #1e2d7d;" &gt;&lt;strong&gt;Disclaimer:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;p&gt;The product information displayed on this website is for your reference only. Hence we request you to always read labels, warnings &amp;amp; directions before using or introducing the food product to your baby. For additional information please refer the product manufacturer’s website.&lt;/p&gt;
+&lt;/div&gt;
+&lt;div&gt;&lt;br&gt;&lt;/div&gt;
+&lt;p&gt;&lt;strong&gt;&lt;span style="color: #fa0808;" &gt;&lt;/span&gt;&lt;/strong&gt;&lt;a href="https://www.uyyaala.com/pages/return-policy" data-mce-href="https://www.uyyaala.com/pages/return-policy"&gt;&lt;strong&gt;&lt;span &gt;&lt;span style="color: #1e2d7d;" &gt;Return Policy:&lt;/span&gt; &lt;/span&gt;&lt;span style="color: #f50b0b;" &gt;Click Here&lt;/span&gt;&lt;/strong&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Cow &amp; Gate</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Infant Formula</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>cow-gate-infant-milk-formula-with-omega-3-stage-2-800g-6m</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Cow &amp; Gate First Infant Baby Milk Formula - Stage 1, 800gms, 0+months</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>&lt;div&gt;
 &lt;div&gt;
 &lt;ul&gt;
-&lt;li&gt;
-&lt;span&gt;&lt;span&gt;Nutritionally complete&lt;span&gt; Follow-on Baby Milk Formula&lt;/span&gt;&lt;/span&gt;&lt;/span&gt;&lt;br&gt;
-&lt;/li&gt;
-&lt;li&gt;&lt;span &gt;Contains Lactose, Milk, Vegetable oils, Maltodextrin, Calcium &amp;amp; more&lt;/span&gt;&lt;/li&gt;
-&lt;li&gt;Suitable as a sole source of nutrition for growing babies&lt;/li&gt;
-&lt;li&gt;Nutritionally complete Fortified Milk Drink&lt;/li&gt;
-&lt;li&gt;Supports your baby’s normal growth and development.&lt;span style="font-size: 11.6667px;" data-mce-style="font-size: 11.6667px;"&gt; &lt;/span&gt;
+&lt;li&gt;Easy-to-digest&lt;span&gt; &lt;/span&gt;&lt;span &gt;Infant Baby Milk Formula&lt;/span&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;span &gt;Contains Whey protein, Vegetable oils, Glucose, GOS from milk &amp;amp; more&lt;/span&gt;&lt;/li&gt;
+&lt;li&gt;Suitable as a sole source of nutrition from child birth&lt;/li&gt;
+&lt;li&gt;Nutritionally complete breast milk substitute&lt;/li&gt;
+&lt;li&gt;Supports your baby’s normal growth and development.&lt;span style="font-size: 11.6667px;"&gt; &lt;/span&gt;
 &lt;/li&gt;
 &lt;li&gt;Contains no artificial sweeteners &amp;amp; flavors&lt;/li&gt;
 &lt;/ul&gt;
-&lt;p&gt;&lt;span style="color: #1e2e7d;" &gt;&lt;strong&gt;Expiry Date :&lt;/strong&gt; 05/2024&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&lt;b&gt;&lt;span style="color: #1e2e7d;" &gt;Return&lt;/span&gt;&lt;span&gt;&lt;span style="color: #ff0000;" &gt;*&lt;/span&gt; &lt;/span&gt;&lt;/b&gt;: No&lt;/p&gt;
-&lt;p&gt;&lt;span&gt;&lt;b&gt;&lt;span style="color: #1e2e7d;" &gt;Replace / Exchange&lt;/span&gt;&lt;span style="color: #ff0000;" &gt;*&lt;/span&gt;&lt;/b&gt;&lt;/span&gt;&lt;span&gt; &lt;/span&gt;: No&lt;/p&gt;
-&lt;p&gt;&lt;span style="color: #1e2e7d;" &gt;&lt;strong&gt;Specifications:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;p&gt;&lt;span style="color: #1e2e7d;"&gt;&lt;strong&gt;Expiry Date :&lt;/strong&gt; 10/2024&lt;/span&gt;&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;&lt;span style="color: #1e2e7d;"&gt;Return&lt;/span&gt;&lt;span&gt;&lt;span style="color: #ff0000;"&gt;*&lt;/span&gt; &lt;/span&gt;&lt;/b&gt;: No&lt;/p&gt;
+&lt;p&gt;&lt;span&gt;&lt;b&gt;&lt;span style="color: #1e2e7d;"&gt;Replace / Exchange&lt;/span&gt;&lt;span style="color: #ff0000;"&gt;*&lt;/span&gt;&lt;/b&gt;&lt;/span&gt;&lt;span&gt; &lt;/span&gt;: No&lt;/p&gt;
+&lt;p&gt;&lt;span style="color: #1e2e7d;"&gt;&lt;strong&gt;Specifications:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
 &lt;ul&gt;
 &lt;li&gt;Brand - Cow &amp;amp; Gate&lt;/li&gt;
-&lt;li&gt;Product - &lt;span &gt;Follow-on Baby Milk Formula&lt;/span&gt;
-&lt;/li&gt;
-&lt;li&gt;Age - 6+months&lt;/li&gt;
-&lt;li&gt;Grams - 800gms&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;&lt;span style="color: #1e2e7d;" &gt;&lt;strong&gt;Instructions:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;/div&gt;
-&lt;ul&gt;
-&lt;li&gt;Consult Doctor before introducing&lt;span&gt; Follow-on Baby Milk Formula&lt;/span&gt;&lt;span &gt;&lt;span&gt; &lt;/span&gt;&lt;/span&gt;to your child&lt;/li&gt;
+&lt;li&gt;Product - First Infant Baby Milk Formula&lt;/li&gt;
+&lt;li&gt;Age - 0+months&lt;/li&gt;
+&lt;li&gt;Item Weight - 800gms&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;&lt;span style="color: #1e2e7d;"&gt;&lt;strong&gt;Instructions:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;/div&gt;
+&lt;ul&gt;
+&lt;li&gt;Consult Doctor before introducing&lt;span&gt; First Infant Baby Milk Formula&lt;/span&gt;&lt;span &gt;&lt;span&gt; &lt;/span&gt;&lt;/span&gt;to your child&lt;/li&gt;
 &lt;li&gt;Do not use fewer scoops than directed&lt;/li&gt;
 &lt;li&gt;Store in cool air tight container&lt;/li&gt;
 &lt;li&gt;Please note : Mothers milk is always best for your baby&lt;/li&gt;
 &lt;/ul&gt;
 &lt;p&gt;Country of Origin: U.K&lt;/p&gt;
-&lt;p&gt;&lt;span style="color: #1e2d7d;" &gt;&lt;strong&gt;Disclaimer:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
+&lt;p&gt;&lt;span style="color: #1e2d7d;"&gt;&lt;strong&gt;Disclaimer:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
 &lt;p&gt;The product information displayed on this website is for your reference only. Hence we request you to always read labels, warnings &amp;amp; directions before using or introducing the food product to your baby. For additional information please refer the product manufacturer’s website.&lt;/p&gt;
 &lt;/div&gt;
-&lt;div&gt;&lt;br&gt;&lt;/div&gt;
-&lt;p&gt;&lt;strong&gt;&lt;span style="color: #fa0808;" &gt;&lt;/span&gt;&lt;/strong&gt;&lt;a href="https://www.uyyaala.com/pages/return-policy" data-mce-href="https://www.uyyaala.com/pages/return-policy"&gt;&lt;strong&gt;&lt;span &gt;&lt;span style="color: #1e2d7d;" &gt;Return Policy:&lt;/span&gt; &lt;/span&gt;&lt;span style="color: #f50b0b;" &gt;Click Here&lt;/span&gt;&lt;/strong&gt;&lt;/a&gt;&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+&lt;div&gt;&lt;/div&gt;
+&lt;p&gt;&lt;strong&gt;&lt;span style="color: #fa0808;"&gt;&lt;/span&gt;&lt;/strong&gt;&lt;a href="https://www.uyyaala.com/pages/return-policy"&gt;&lt;strong&gt;&lt;span &gt;&lt;span style="color: #1e2d7d;"&gt;Return Policy:&lt;/span&gt; &lt;/span&gt;&lt;span style="color: #f50b0b;"&gt;Click Here&lt;/span&gt;&lt;/strong&gt;&lt;/a&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Cow &amp; Gate</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Infant Formula</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>cow-gate-first-infant-baby-milk-formula-stage-1-800gms-0-months</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Cow &amp; Gate</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Infant Formula</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>cow-gate-infant-milk-formula-with-omega-3-stage-2-800g-6m</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Cow &amp; Gate First Infant Baby Milk Formula - Stage 1, 800gms, 0+months</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>&lt;div&gt;
-&lt;div&gt;
-&lt;ul&gt;
-&lt;li&gt;Easy-to-digest&lt;span&gt; &lt;/span&gt;&lt;span &gt;Infant Baby Milk Formula&lt;/span&gt;
-&lt;/li&gt;
-&lt;li&gt;&lt;span &gt;Contains Whey protein, Vegetable oils, Glucose, GOS from milk &amp;amp; more&lt;/span&gt;&lt;/li&gt;
-&lt;li&gt;Suitable as a sole source of nutrition from child birth&lt;/li&gt;
-&lt;li&gt;Nutritionally complete breast milk substitute&lt;/li&gt;
-&lt;li&gt;Supports your baby’s normal growth and development.&lt;span style="font-size: 11.6667px;"&gt; &lt;/span&gt;
-&lt;/li&gt;
-&lt;li&gt;Contains no artificial sweeteners &amp;amp; flavors&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;&lt;span style="color: #1e2e7d;"&gt;&lt;strong&gt;Expiry Date :&lt;/strong&gt; 10/2024&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;&lt;b&gt;&lt;span style="color: #1e2e7d;"&gt;Return&lt;/span&gt;&lt;span&gt;&lt;span style="color: #ff0000;"&gt;*&lt;/span&gt; &lt;/span&gt;&lt;/b&gt;: No&lt;/p&gt;
-&lt;p&gt;&lt;span&gt;&lt;b&gt;&lt;span style="color: #1e2e7d;"&gt;Replace / Exchange&lt;/span&gt;&lt;span style="color: #ff0000;"&gt;*&lt;/span&gt;&lt;/b&gt;&lt;/span&gt;&lt;span&gt; &lt;/span&gt;: No&lt;/p&gt;
-&lt;p&gt;&lt;span style="color: #1e2e7d;"&gt;&lt;strong&gt;Specifications:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;Brand - Cow &amp;amp; Gate&lt;/li&gt;
-&lt;li&gt;Product - First Infant Baby Milk Formula&lt;/li&gt;
-&lt;li&gt;Age - 0+months&lt;/li&gt;
-&lt;li&gt;Item Weight - 800gms&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;&lt;span style="color: #1e2e7d;"&gt;&lt;strong&gt;Instructions:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;/div&gt;
-&lt;ul&gt;
-&lt;li&gt;Consult Doctor before introducing&lt;span&gt; First Infant Baby Milk Formula&lt;/span&gt;&lt;span &gt;&lt;span&gt; &lt;/span&gt;&lt;/span&gt;to your child&lt;/li&gt;
-&lt;li&gt;Do not use fewer scoops than directed&lt;/li&gt;
-&lt;li&gt;Store in cool air tight container&lt;/li&gt;
-&lt;li&gt;Please note : Mothers milk is always best for your baby&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;Country of Origin: U.K&lt;/p&gt;
-&lt;p&gt;&lt;span style="color: #1e2d7d;"&gt;&lt;strong&gt;Disclaimer:&lt;/strong&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;p&gt;The product information displayed on this website is for your reference only. Hence we request you to always read labels, warnings &amp;amp; directions before using or introducing the food product to your baby. For additional information please refer the product manufacturer’s website.&lt;/p&gt;
-&lt;/div&gt;
-&lt;div&gt;&lt;/div&gt;
-&lt;p&gt;&lt;strong&gt;&lt;span style="color: #fa0808;"&gt;&lt;/span&gt;&lt;/strong&gt;&lt;a href="https://www.uyyaala.com/pages/return-policy"&gt;&lt;strong&gt;&lt;span &gt;&lt;span style="color: #1e2d7d;"&gt;Return Policy:&lt;/span&gt; &lt;/span&gt;&lt;span style="color: #f50b0b;"&gt;Click Here&lt;/span&gt;&lt;/strong&gt;&lt;/a&gt;&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Cow &amp; Gate</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Infant Formula</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>cow-gate-first-infant-baby-milk-formula-stage-1-800gms-0-months</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Cow &amp; Gate Fortified Toddler Baby Milk Formula - Stage 3, 800gms, 1+years</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>&lt;div&gt;
 &lt;div&gt;
@@ -731,72 +641,32 @@
 &lt;p&gt;&lt;strong&gt;&lt;span style="color: #fa0808;"&gt;&lt;/span&gt;&lt;/strong&gt;&lt;a href="https://www.uyyaala.com/pages/return-policy"&gt;&lt;strong&gt;&lt;span &gt;&lt;span style="color: #1e2d7d;"&gt;Return Policy:&lt;/span&gt; &lt;/span&gt;&lt;span style="color: #f50b0b;"&gt;Click Here&lt;/span&gt;&lt;/strong&gt;&lt;/a&gt;&lt;/p&gt;</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Cow &amp; Gate</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Infant Formula</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>cow-gate-fortified-toddler-baby-milk-formula-stage-3-800gms-1-years</t>
+        </is>
+      </c>
     </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Cow &amp; Gate</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Infant Formula</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>cow-gate-fortified-toddler-baby-milk-formula-stage-3-800gms-1-years</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>Cow &amp; Gate Fortified Toddler Baby Milk Formula - Stage 4, 800gms, 2+years</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>&lt;div&gt;
 &lt;div&gt;
@@ -836,72 +706,32 @@
 &lt;p&gt;&lt;strong&gt;&lt;span style="color: #fa0808;"&gt;&lt;/span&gt;&lt;/strong&gt;&lt;a href="https://www.uyyaala.com/pages/return-policy"&gt;&lt;strong&gt;&lt;span &gt;&lt;span style="color: #1e2d7d;"&gt;Return Policy:&lt;/span&gt; &lt;/span&gt;&lt;span style="color: #f50b0b;"&gt;Click Here&lt;/span&gt;&lt;/strong&gt;&lt;/a&gt;&lt;/p&gt;</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Cow &amp; Gate</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Infant Formula</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>cow-gate-fortified-toddler-baby-milk-formula-stage-4-800gms-2-years</t>
+        </is>
+      </c>
     </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Cow &amp; Gate</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Infant Formula</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>cow-gate-fortified-toddler-baby-milk-formula-stage-4-800gms-2-years</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Cow &amp; Gate Comfort from Birth Infant Baby Milk Formula, 800gms, 0+months</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>&lt;div&gt;
 &lt;div&gt;
@@ -942,72 +772,32 @@
 &lt;p&gt;&lt;strong&gt;&lt;span style="color: #fa0808;"&gt;&lt;/span&gt;&lt;/strong&gt;&lt;a href="https://www.uyyaala.com/pages/return-policy"&gt;&lt;strong&gt;&lt;span &gt;&lt;span style="color: #1e2d7d;"&gt;Return Policy:&lt;/span&gt; &lt;/span&gt;&lt;span style="color: #f50b0b;"&gt;Click Here&lt;/span&gt;&lt;/strong&gt;&lt;/a&gt;&lt;/p&gt;</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Cow &amp; Gate</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Infant Formula</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>cow-gate-comfort-from-birth-infant-baby-milk-formula-800gms-0-months</t>
+        </is>
+      </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Cow &amp; Gate</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Infant Formula</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>cow-gate-comfort-from-birth-infant-baby-milk-formula-800gms-0-months</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Cow &amp; Gate Anti-Reflux from Birth Infant Baby Milk Formula, 800gms, 0 to 12months</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>&lt;div&gt;
 &lt;div&gt;
@@ -1051,47 +841,17 @@
 &lt;p&gt;&lt;strong&gt;&lt;span style="color: #fa0808;" &gt;&lt;/span&gt;&lt;/strong&gt;&lt;a href="https://www.uyyaala.com/pages/return-policy" data-mce-href="https://www.uyyaala.com/pages/return-policy"&gt;&lt;strong&gt;&lt;span &gt;&lt;span style="color: #1e2d7d;" &gt;Return Policy:&lt;/span&gt; &lt;/span&gt;&lt;span style="color: #f50b0b;" &gt;Click Here&lt;/span&gt;&lt;/strong&gt;&lt;/a&gt;&lt;/p&gt;</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr"/>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Cow &amp; Gate</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>Infant Formula</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>cow-gate-anti-reflux-from-birth-infant-baby-milk-formula-800gms-0-months</t>
         </is>

</xml_diff>